<commit_message>
Implement File Upload with AutoIT
</commit_message>
<xml_diff>
--- a/MarsFramework/ExcelData/TestData.xlsx
+++ b/MarsFramework/ExcelData/TestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\MarsProject\marsframework\MarsFramework\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1C2ED17-89B5-4538-9088-41C4EEFE1B17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B2F82A-6A99-46A3-9A41-8B05B6F8105A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -823,7 +823,7 @@
   <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +916,7 @@
         <v>52</v>
       </c>
       <c r="H2" s="3">
-        <v>44109</v>
+        <v>44119</v>
       </c>
       <c r="I2" s="3">
         <v>44127</v>
@@ -966,7 +966,7 @@
         <v>52</v>
       </c>
       <c r="H3" s="3">
-        <v>44109</v>
+        <v>44119</v>
       </c>
       <c r="I3" s="3">
         <v>44127</v>

</xml_diff>